<commit_message>
prep to add player stats to xlsx
</commit_message>
<xml_diff>
--- a/2018/league/alpha/data/standings/2018_week_1_standings.xlsx
+++ b/2018/league/alpha/data/standings/2018_week_1_standings.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Standings" sheetId="1" r:id="rId1"/>
     <sheet name="Points System" sheetId="2" r:id="rId2"/>
-    <sheet name="Weekly Player Stats" sheetId="3" r:id="rId3"/>
+    <sheet name="Weekly Player Points" sheetId="3" r:id="rId3"/>
     <sheet name="Week 1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -163,40 +163,154 @@
     <t>Free Agent</t>
   </si>
   <si>
+    <t>M.Dickson</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>B.Colquitt</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>A.Lee</t>
+  </si>
+  <si>
+    <t>ARI</t>
+  </si>
+  <si>
+    <t>M.Palardy</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>D.Colquitt</t>
+  </si>
+  <si>
+    <t>KC</t>
+  </si>
+  <si>
+    <t>S.Koch</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
     <t>C.Johnston</t>
   </si>
   <si>
     <t>PHI</t>
   </si>
   <si>
+    <t>R.Allen</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>M.King</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>B.Kern</t>
+  </si>
+  <si>
+    <t>TEN</t>
+  </si>
+  <si>
+    <t>M.Wile</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>C.Bojorquez</t>
+  </si>
+  <si>
+    <t>BUF</t>
+  </si>
+  <si>
+    <t>C.Jones</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>T.Daniel</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>L.Cooke</t>
+  </si>
+  <si>
+    <t>JAX</t>
+  </si>
+  <si>
+    <t>J.Berry</t>
+  </si>
+  <si>
+    <t>PIT</t>
+  </si>
+  <si>
+    <t>R.Dixon</t>
+  </si>
+  <si>
+    <t>NYG</t>
+  </si>
+  <si>
+    <t>T.Way</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>M.Haack</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
     <t>M.Bosher</t>
   </si>
   <si>
     <t>ATL</t>
   </si>
   <si>
-    <t>C.Bojorquez</t>
-  </si>
-  <si>
-    <t>BUF</t>
-  </si>
-  <si>
-    <t>S.Koch</t>
-  </si>
-  <si>
-    <t>BAL</t>
-  </si>
-  <si>
-    <t>J.Berry</t>
-  </si>
-  <si>
-    <t>PIT</t>
-  </si>
-  <si>
-    <t>B.Colquitt</t>
-  </si>
-  <si>
-    <t>CLE</t>
+    <t>P.O'Donnell</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>T.Morstead</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>K.Huber</t>
+  </si>
+  <si>
+    <t>CIN</t>
+  </si>
+  <si>
+    <t>J.Scott</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>B.Pinion</t>
+  </si>
+  <si>
+    <t>SF</t>
   </si>
   <si>
     <t>R.Sanchez</t>
@@ -205,69 +319,9 @@
     <t>IND</t>
   </si>
   <si>
-    <t>K.Huber</t>
-  </si>
-  <si>
-    <t>CIN</t>
-  </si>
-  <si>
-    <t>M.Haack</t>
-  </si>
-  <si>
-    <t>MIA</t>
-  </si>
-  <si>
-    <t>B.Kern</t>
-  </si>
-  <si>
-    <t>TEN</t>
-  </si>
-  <si>
-    <t>B.Pinion</t>
-  </si>
-  <si>
-    <t>SF</t>
-  </si>
-  <si>
-    <t>M.Wile</t>
-  </si>
-  <si>
-    <t>MIN</t>
-  </si>
-  <si>
-    <t>R.Allen</t>
-  </si>
-  <si>
-    <t>NE</t>
-  </si>
-  <si>
-    <t>T.Daniel</t>
-  </si>
-  <si>
-    <t>HOU</t>
-  </si>
-  <si>
-    <t>T.Morstead</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>B.Anger</t>
   </si>
   <si>
-    <t>R.Dixon</t>
-  </si>
-  <si>
-    <t>NYG</t>
-  </si>
-  <si>
-    <t>L.Cooke</t>
-  </si>
-  <si>
-    <t>JAX</t>
-  </si>
-  <si>
     <t>D.Kaser</t>
   </si>
   <si>
@@ -275,60 +329,6 @@
   </si>
   <si>
     <t>C.Sturgis</t>
-  </si>
-  <si>
-    <t>D.Colquitt</t>
-  </si>
-  <si>
-    <t>KC</t>
-  </si>
-  <si>
-    <t>T.Way</t>
-  </si>
-  <si>
-    <t>WAS</t>
-  </si>
-  <si>
-    <t>A.Lee</t>
-  </si>
-  <si>
-    <t>ARI</t>
-  </si>
-  <si>
-    <t>C.Jones</t>
-  </si>
-  <si>
-    <t>DAL</t>
-  </si>
-  <si>
-    <t>M.Palardy</t>
-  </si>
-  <si>
-    <t>CAR</t>
-  </si>
-  <si>
-    <t>M.King</t>
-  </si>
-  <si>
-    <t>DEN</t>
-  </si>
-  <si>
-    <t>M.Dickson</t>
-  </si>
-  <si>
-    <t>SEA</t>
-  </si>
-  <si>
-    <t>J.Scott</t>
-  </si>
-  <si>
-    <t>GB</t>
-  </si>
-  <si>
-    <t>P.O'Donnell</t>
-  </si>
-  <si>
-    <t>CHI</t>
   </si>
 </sst>
 </file>
@@ -1073,46 +1073,46 @@
         <v>0</v>
       </c>
       <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>5</v>
+      </c>
+      <c r="J2" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>4</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="R2" s="4">
         <v>0.4</v>
       </c>
-      <c r="G2" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="I2" s="4">
-        <v>4</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4">
-        <v>1</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
-        <v>0</v>
-      </c>
-      <c r="P2" s="4">
-        <v>0.7166666666666665</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="R2" s="4">
-        <v>0.2</v>
-      </c>
       <c r="S2" s="4">
-        <v>-0</v>
+        <v>-0.25</v>
       </c>
       <c r="T2" s="4">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="Y2" s="4">
-        <v>7.766666666666667</v>
+        <v>15.45</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1150,16 +1150,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G3" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="4">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3" s="4">
         <v>0</v>
@@ -1168,10 +1168,10 @@
         <v>0</v>
       </c>
       <c r="L3" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M3" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N3" s="4">
         <v>0</v>
@@ -1180,16 +1180,16 @@
         <v>0</v>
       </c>
       <c r="P3" s="4">
-        <v>0.2666666666666664</v>
+        <v>-0.15</v>
       </c>
       <c r="Q3" s="4">
-        <v>0.175</v>
+        <v>-0.2199999999999999</v>
       </c>
       <c r="R3" s="4">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="S3" s="4">
-        <v>-0.25</v>
+        <v>-0</v>
       </c>
       <c r="T3" s="4">
         <v>0</v>
@@ -1207,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="Y3" s="4">
-        <v>3.641666666666667</v>
+        <v>11.63</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1227,19 +1227,19 @@
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G4" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I4" s="4">
         <v>4</v>
       </c>
       <c r="J4" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K4" s="4">
         <v>0</v>
@@ -1248,7 +1248,7 @@
         <v>3</v>
       </c>
       <c r="M4" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N4" s="4">
         <v>0</v>
@@ -1257,16 +1257,16 @@
         <v>0</v>
       </c>
       <c r="P4" s="4">
-        <v>0.4625</v>
+        <v>0.7600000000000002</v>
       </c>
       <c r="Q4" s="4">
-        <v>-0.1800000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="R4" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="4">
-        <v>-0.25</v>
+        <v>-0</v>
       </c>
       <c r="T4" s="4">
         <v>0</v>
@@ -1275,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="V4" s="4">
-        <v>-1.5</v>
+        <v>-0</v>
       </c>
       <c r="W4" s="4">
         <v>-0</v>
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="Y4" s="4">
-        <v>6.0825</v>
+        <v>10.46</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1304,19 +1304,19 @@
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G5" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H5" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J5" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K5" s="4">
         <v>0</v>
@@ -1325,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="M5" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N5" s="4">
         <v>0</v>
@@ -1334,16 +1334,16 @@
         <v>0</v>
       </c>
       <c r="P5" s="4">
-        <v>0.6399999999999999</v>
+        <v>0.2833333333333336</v>
       </c>
       <c r="Q5" s="4">
-        <v>0.2666666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="R5" s="4">
-        <v>0.7000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="S5" s="4">
-        <v>-0</v>
+        <v>-0.25</v>
       </c>
       <c r="T5" s="4">
         <v>0</v>
@@ -1361,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="Y5" s="4">
-        <v>8.456666666666665</v>
+        <v>10.38333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1384,16 +1384,16 @@
         <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="H6" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="4">
         <v>2</v>
       </c>
       <c r="J6" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K6" s="4">
         <v>0</v>
@@ -1402,25 +1402,25 @@
         <v>3</v>
       </c>
       <c r="M6" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N6" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O6" s="4">
         <v>0</v>
       </c>
       <c r="P6" s="4">
-        <v>-0.5714285714285715</v>
+        <v>0.6200000000000003</v>
       </c>
       <c r="Q6" s="4">
-        <v>-0.6000000000000001</v>
+        <v>1.15</v>
       </c>
       <c r="R6" s="4">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="S6" s="4">
-        <v>-0.25</v>
+        <v>-0</v>
       </c>
       <c r="T6" s="4">
         <v>0</v>
@@ -1438,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="Y6" s="4">
-        <v>4.728571428571429</v>
+        <v>10.27</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1458,28 +1458,28 @@
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="I7" s="4">
         <v>3</v>
       </c>
       <c r="J7" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K7" s="4">
         <v>0</v>
       </c>
       <c r="L7" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M7" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N7" s="4">
         <v>0</v>
@@ -1488,13 +1488,13 @@
         <v>0</v>
       </c>
       <c r="P7" s="4">
-        <v>-0.15</v>
+        <v>0.6399999999999999</v>
       </c>
       <c r="Q7" s="4">
-        <v>-0.2199999999999999</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="R7" s="4">
-        <v>0.3</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="S7" s="4">
         <v>-0</v>
@@ -1515,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="Y7" s="4">
-        <v>11.63</v>
+        <v>8.456666666666665</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1535,25 +1535,25 @@
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G8" s="4">
         <v>0.25</v>
       </c>
       <c r="H8" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I8" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J8" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K8" s="4">
         <v>0</v>
       </c>
       <c r="L8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="4">
         <v>0</v>
@@ -1565,16 +1565,16 @@
         <v>0</v>
       </c>
       <c r="P8" s="4">
-        <v>0.25</v>
+        <v>0.7166666666666665</v>
       </c>
       <c r="Q8" s="4">
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="R8" s="4">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="S8" s="4">
-        <v>-0.25</v>
+        <v>-0</v>
       </c>
       <c r="T8" s="4">
         <v>0</v>
@@ -1592,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="Y8" s="4">
-        <v>1.75</v>
+        <v>7.766666666666667</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1615,13 +1615,13 @@
         <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H9" s="4">
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="4">
         <v>0</v>
@@ -1630,22 +1630,22 @@
         <v>0</v>
       </c>
       <c r="L9" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M9" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N9" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O9" s="4">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="P9" s="4">
-        <v>0.3</v>
+        <v>0.1833333333333336</v>
       </c>
       <c r="Q9" s="4">
-        <v>0.9</v>
+        <v>-0.1</v>
       </c>
       <c r="R9" s="4">
         <v>0.5</v>
@@ -1669,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="Y9" s="4">
-        <v>2.7</v>
+        <v>7.083333333333334</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1689,28 +1689,28 @@
         <v>0</v>
       </c>
       <c r="F10" s="4">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
       </c>
       <c r="H10" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I10" s="4">
         <v>2</v>
       </c>
       <c r="J10" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K10" s="4">
         <v>0</v>
       </c>
       <c r="L10" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M10" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N10" s="4">
         <v>0</v>
@@ -1719,10 +1719,10 @@
         <v>0</v>
       </c>
       <c r="P10" s="4">
-        <v>0.875</v>
+        <v>-0.05</v>
       </c>
       <c r="Q10" s="4">
-        <v>-1.3</v>
+        <v>0.5333333333333334</v>
       </c>
       <c r="R10" s="4">
         <v>0.5</v>
@@ -1746,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="Y10" s="4">
-        <v>4.375</v>
+        <v>6.933333333333334</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1849,10 +1849,10 @@
         <v>0.25</v>
       </c>
       <c r="H12" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="4">
         <v>0</v>
@@ -1861,25 +1861,25 @@
         <v>0</v>
       </c>
       <c r="L12" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M12" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N12" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O12" s="4">
         <v>0</v>
       </c>
       <c r="P12" s="4">
-        <v>-0.15</v>
+        <v>-0.6666666666666665</v>
       </c>
       <c r="Q12" s="4">
-        <v>0.6666666666666666</v>
+        <v>0.2</v>
       </c>
       <c r="R12" s="4">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="S12" s="4">
         <v>-0</v>
@@ -1900,7 +1900,7 @@
         <v>0</v>
       </c>
       <c r="Y12" s="4">
-        <v>2.166666666666667</v>
+        <v>6.433333333333334</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1926,40 +1926,40 @@
         <v>0.25</v>
       </c>
       <c r="H13" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="4">
+        <v>4</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>3</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <v>0.4625</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>-0.1800000000000001</v>
+      </c>
+      <c r="R13" s="4">
         <v>0.1</v>
       </c>
-      <c r="I13" s="4">
-        <v>1</v>
-      </c>
-      <c r="J13" s="4">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <v>4</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="4">
-        <v>-0.6666666666666665</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="R13" s="4">
-        <v>0.3</v>
-      </c>
       <c r="S13" s="4">
-        <v>-0</v>
+        <v>-0.25</v>
       </c>
       <c r="T13" s="4">
         <v>0</v>
@@ -1968,7 +1968,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="4">
-        <v>-0</v>
+        <v>-1.5</v>
       </c>
       <c r="W13" s="4">
         <v>-0</v>
@@ -1977,7 +1977,7 @@
         <v>0</v>
       </c>
       <c r="Y13" s="4">
-        <v>6.433333333333334</v>
+        <v>6.0825</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2000,13 +2000,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H14" s="4">
         <v>0</v>
       </c>
       <c r="I14" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J14" s="4">
         <v>0</v>
@@ -2018,25 +2018,25 @@
         <v>2</v>
       </c>
       <c r="M14" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N14" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O14" s="4">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="P14" s="4">
-        <v>0.1833333333333336</v>
+        <v>0.3833333333333336</v>
       </c>
       <c r="Q14" s="4">
-        <v>-0.1</v>
+        <v>-0.65</v>
       </c>
       <c r="R14" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S14" s="4">
-        <v>-0</v>
+        <v>-0.25</v>
       </c>
       <c r="T14" s="4">
         <v>0</v>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="Y14" s="4">
-        <v>7.083333333333334</v>
+        <v>5.983333333333333</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2154,13 +2154,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H16" s="4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I16" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
@@ -2169,7 +2169,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M16" s="4">
         <v>0</v>
@@ -2181,13 +2181,13 @@
         <v>0</v>
       </c>
       <c r="P16" s="4">
-        <v>0.7000000000000001</v>
+        <v>-0.7285714285714285</v>
       </c>
       <c r="Q16" s="4">
-        <v>0.2666666666666667</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="R16" s="4">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="S16" s="4">
         <v>-0</v>
@@ -2208,7 +2208,7 @@
         <v>0</v>
       </c>
       <c r="Y16" s="4">
-        <v>3.366666666666667</v>
+        <v>4.788095238095238</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2222,32 +2222,32 @@
         <v>78</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
         <v>3</v>
       </c>
-      <c r="E17" s="4">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <v>0</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4">
-        <v>0</v>
-      </c>
       <c r="M17" s="4">
         <v>0</v>
       </c>
@@ -2258,13 +2258,13 @@
         <v>0</v>
       </c>
       <c r="P17" s="4">
-        <v>-0.3</v>
+        <v>-0.5714285714285715</v>
       </c>
       <c r="Q17" s="4">
-        <v>0.9</v>
+        <v>-0.6000000000000001</v>
       </c>
       <c r="R17" s="4">
-        <v>0.7000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="S17" s="4">
         <v>-0.25</v>
@@ -2285,7 +2285,7 @@
         <v>0</v>
       </c>
       <c r="Y17" s="4">
-        <v>1.05</v>
+        <v>4.728571428571429</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2296,10 +2296,10 @@
         <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="4">
         <v>0</v>
@@ -2373,10 +2373,10 @@
         <v>47</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E19" s="4">
         <v>0</v>
@@ -2385,13 +2385,13 @@
         <v>0</v>
       </c>
       <c r="G19" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H19" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I19" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19" s="4">
         <v>0</v>
@@ -2400,10 +2400,10 @@
         <v>0</v>
       </c>
       <c r="L19" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M19" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N19" s="4">
         <v>0</v>
@@ -2412,13 +2412,13 @@
         <v>0</v>
       </c>
       <c r="P19" s="4">
-        <v>-0.7285714285714285</v>
+        <v>0.15</v>
       </c>
       <c r="Q19" s="4">
-        <v>0.7666666666666667</v>
+        <v>-1.3</v>
       </c>
       <c r="R19" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="S19" s="4">
         <v>-0</v>
@@ -2439,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="Y19" s="4">
-        <v>4.788095238095238</v>
+        <v>4.500000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2450,16 +2450,16 @@
         <v>47</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E20" s="4">
         <v>0</v>
       </c>
       <c r="F20" s="4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G20" s="4">
         <v>0</v>
@@ -2471,7 +2471,7 @@
         <v>2</v>
       </c>
       <c r="J20" s="4">
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="K20" s="4">
         <v>0</v>
@@ -2489,16 +2489,16 @@
         <v>0</v>
       </c>
       <c r="P20" s="4">
-        <v>1.5</v>
+        <v>0.875</v>
       </c>
       <c r="Q20" s="4">
-        <v>-3.85</v>
+        <v>-1.3</v>
       </c>
       <c r="R20" s="4">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="S20" s="4">
-        <v>-0.25</v>
+        <v>-0</v>
       </c>
       <c r="T20" s="4">
         <v>0</v>
@@ -2516,7 +2516,7 @@
         <v>0</v>
       </c>
       <c r="Y20" s="4">
-        <v>0.3499999999999999</v>
+        <v>4.375</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -2527,10 +2527,10 @@
         <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
@@ -2539,13 +2539,13 @@
         <v>0</v>
       </c>
       <c r="G21" s="4">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H21" s="4">
         <v>0</v>
       </c>
       <c r="I21" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="4">
         <v>0</v>
@@ -2566,10 +2566,10 @@
         <v>0</v>
       </c>
       <c r="P21" s="4">
-        <v>-2.1</v>
+        <v>0.2666666666666664</v>
       </c>
       <c r="Q21" s="4">
-        <v>0</v>
+        <v>0.175</v>
       </c>
       <c r="R21" s="4">
         <v>0.2</v>
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="Y21" s="4">
-        <v>-1.15</v>
+        <v>3.641666666666667</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -2604,10 +2604,10 @@
         <v>47</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E22" s="4">
         <v>0</v>
@@ -2616,40 +2616,40 @@
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="H22" s="4">
         <v>0</v>
       </c>
       <c r="I22" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J22" s="4">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="K22" s="4">
         <v>0</v>
       </c>
       <c r="L22" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M22" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N22" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O22" s="4">
         <v>0</v>
       </c>
       <c r="P22" s="4">
-        <v>0.6200000000000003</v>
+        <v>0.525</v>
       </c>
       <c r="Q22" s="4">
-        <v>1.15</v>
+        <v>-0.8</v>
       </c>
       <c r="R22" s="4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S22" s="4">
         <v>-0</v>
@@ -2670,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="Y22" s="4">
-        <v>10.27</v>
+        <v>3.625</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2681,10 +2681,10 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E23" s="4">
         <v>0</v>
@@ -2693,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H23" s="4">
         <v>0</v>
@@ -2708,10 +2708,10 @@
         <v>0</v>
       </c>
       <c r="L23" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M23" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N23" s="4">
         <v>0</v>
@@ -2720,10 +2720,10 @@
         <v>0</v>
       </c>
       <c r="P23" s="4">
-        <v>0.15</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="Q23" s="4">
-        <v>-1.3</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="R23" s="4">
         <v>0.4</v>
@@ -2747,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="Y23" s="4">
-        <v>4.500000000000001</v>
+        <v>3.366666666666667</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2758,53 +2758,53 @@
         <v>47</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E24" s="4">
         <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>1</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0</v>
+      </c>
+      <c r="O24" s="4">
+        <v>0</v>
+      </c>
+      <c r="P24" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="R24" s="4">
         <v>0.5</v>
       </c>
-      <c r="H24" s="4">
-        <v>0</v>
-      </c>
-      <c r="I24" s="4">
-        <v>4</v>
-      </c>
-      <c r="J24" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="K24" s="4">
-        <v>0</v>
-      </c>
-      <c r="L24" s="4">
-        <v>3</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="N24" s="4">
-        <v>0</v>
-      </c>
-      <c r="O24" s="4">
-        <v>0</v>
-      </c>
-      <c r="P24" s="4">
-        <v>0.7600000000000002</v>
-      </c>
-      <c r="Q24" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="R24" s="4">
-        <v>0</v>
-      </c>
       <c r="S24" s="4">
         <v>-0</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="Y24" s="4">
-        <v>10.46</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -2835,10 +2835,10 @@
         <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E25" s="4">
         <v>0</v>
@@ -2847,13 +2847,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="4">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H25" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I25" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J25" s="4">
         <v>0</v>
@@ -2862,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M25" s="4">
         <v>0</v>
@@ -2874,16 +2874,16 @@
         <v>0</v>
       </c>
       <c r="P25" s="4">
-        <v>0.3833333333333336</v>
+        <v>0.3</v>
       </c>
       <c r="Q25" s="4">
-        <v>-0.65</v>
+        <v>-1.35</v>
       </c>
       <c r="R25" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S25" s="4">
-        <v>-0.25</v>
+        <v>-0</v>
       </c>
       <c r="T25" s="4">
         <v>0</v>
@@ -2901,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="Y25" s="4">
-        <v>5.983333333333333</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="26" spans="1:25">
@@ -2912,55 +2912,55 @@
         <v>47</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E26" s="4">
         <v>0</v>
       </c>
       <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4">
+        <v>1</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>0</v>
+      </c>
+      <c r="O26" s="4">
+        <v>0</v>
+      </c>
+      <c r="P26" s="4">
+        <v>-0.15</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="R26" s="4">
         <v>0.4</v>
       </c>
-      <c r="G26" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="H26" s="4">
-        <v>0</v>
-      </c>
-      <c r="I26" s="4">
-        <v>5</v>
-      </c>
-      <c r="J26" s="4">
-        <v>0</v>
-      </c>
-      <c r="K26" s="4">
-        <v>0</v>
-      </c>
-      <c r="L26" s="4">
-        <v>3</v>
-      </c>
-      <c r="M26" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="N26" s="4">
-        <v>0</v>
-      </c>
-      <c r="O26" s="4">
-        <v>0</v>
-      </c>
-      <c r="P26" s="4">
-        <v>0.2833333333333336</v>
-      </c>
-      <c r="Q26" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="R26" s="4">
-        <v>0.2</v>
-      </c>
       <c r="S26" s="4">
-        <v>-0.25</v>
+        <v>-0</v>
       </c>
       <c r="T26" s="4">
         <v>0</v>
@@ -2978,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="Y26" s="4">
-        <v>10.38333333333333</v>
+        <v>2.166666666666667</v>
       </c>
     </row>
     <row r="27" spans="1:25">
@@ -2989,10 +2989,10 @@
         <v>47</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
@@ -3001,13 +3001,13 @@
         <v>0</v>
       </c>
       <c r="G27" s="4">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H27" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27" s="4">
         <v>0</v>
@@ -3016,10 +3016,10 @@
         <v>0</v>
       </c>
       <c r="L27" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M27" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N27" s="4">
         <v>0</v>
@@ -3028,16 +3028,16 @@
         <v>0</v>
       </c>
       <c r="P27" s="4">
-        <v>-0.05</v>
+        <v>0.25</v>
       </c>
       <c r="Q27" s="4">
-        <v>0.5333333333333334</v>
+        <v>1</v>
       </c>
       <c r="R27" s="4">
         <v>0.5</v>
       </c>
       <c r="S27" s="4">
-        <v>-0</v>
+        <v>-0.25</v>
       </c>
       <c r="T27" s="4">
         <v>0</v>
@@ -3055,7 +3055,7 @@
         <v>0</v>
       </c>
       <c r="Y27" s="4">
-        <v>6.933333333333334</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="28" spans="1:25">
@@ -3066,10 +3066,10 @@
         <v>47</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="E28" s="4">
         <v>0</v>
@@ -3081,37 +3081,37 @@
         <v>0</v>
       </c>
       <c r="H28" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I28" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J28" s="4">
-        <v>2.25</v>
+        <v>0</v>
       </c>
       <c r="K28" s="4">
         <v>0</v>
       </c>
       <c r="L28" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M28" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N28" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O28" s="4">
         <v>0</v>
       </c>
       <c r="P28" s="4">
-        <v>1.4</v>
+        <v>-0.3</v>
       </c>
       <c r="Q28" s="4">
-        <v>0.45</v>
+        <v>0.9</v>
       </c>
       <c r="R28" s="4">
-        <v>0.4</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="S28" s="4">
         <v>-0.25</v>
@@ -3132,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="Y28" s="4">
-        <v>15.45</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="29" spans="1:25">
@@ -3143,10 +3143,10 @@
         <v>47</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E29" s="4">
         <v>0</v>
@@ -3155,22 +3155,22 @@
         <v>0</v>
       </c>
       <c r="G29" s="4">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H29" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="4">
         <v>2</v>
       </c>
       <c r="J29" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K29" s="4">
         <v>0</v>
       </c>
       <c r="L29" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" s="4">
         <v>0</v>
@@ -3182,16 +3182,16 @@
         <v>0</v>
       </c>
       <c r="P29" s="4">
-        <v>0.3</v>
+        <v>1.5</v>
       </c>
       <c r="Q29" s="4">
-        <v>-1.35</v>
+        <v>-3.85</v>
       </c>
       <c r="R29" s="4">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="S29" s="4">
-        <v>-0</v>
+        <v>-0.25</v>
       </c>
       <c r="T29" s="4">
         <v>0</v>
@@ -3209,7 +3209,7 @@
         <v>0</v>
       </c>
       <c r="Y29" s="4">
-        <v>2.7</v>
+        <v>0.3499999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -3220,11 +3220,11 @@
         <v>47</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E30" s="4">
         <v>0</v>
       </c>
@@ -3232,16 +3232,16 @@
         <v>0</v>
       </c>
       <c r="G30" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="H30" s="4">
         <v>0</v>
       </c>
       <c r="I30" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" s="4">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K30" s="4">
         <v>0</v>
@@ -3259,16 +3259,16 @@
         <v>0</v>
       </c>
       <c r="P30" s="4">
-        <v>0.525</v>
+        <v>-2.1</v>
       </c>
       <c r="Q30" s="4">
-        <v>-0.8</v>
+        <v>0</v>
       </c>
       <c r="R30" s="4">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="S30" s="4">
-        <v>-0</v>
+        <v>-0.25</v>
       </c>
       <c r="T30" s="4">
         <v>0</v>
@@ -3286,7 +3286,7 @@
         <v>0</v>
       </c>
       <c r="Y30" s="4">
-        <v>3.625</v>
+        <v>-1.15</v>
       </c>
     </row>
   </sheetData>
@@ -3398,10 +3398,10 @@
         <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
@@ -3475,10 +3475,10 @@
         <v>47</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E3" s="4">
         <v>0</v>
@@ -3552,10 +3552,10 @@
         <v>47</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
@@ -3629,10 +3629,10 @@
         <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
@@ -3706,10 +3706,10 @@
         <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
@@ -3783,10 +3783,10 @@
         <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -3860,10 +3860,10 @@
         <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -3937,10 +3937,10 @@
         <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
@@ -4014,10 +4014,10 @@
         <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -4168,10 +4168,10 @@
         <v>47</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E12" s="4">
         <v>0</v>
@@ -4245,10 +4245,10 @@
         <v>47</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -4322,10 +4322,10 @@
         <v>47</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -4476,10 +4476,10 @@
         <v>47</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E16" s="4">
         <v>0</v>
@@ -4553,10 +4553,10 @@
         <v>47</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="E17" s="4">
         <v>0</v>
@@ -4630,10 +4630,10 @@
         <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="4">
         <v>0</v>
@@ -4707,10 +4707,10 @@
         <v>47</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E19" s="4">
         <v>0</v>
@@ -4784,10 +4784,10 @@
         <v>47</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="E20" s="4">
         <v>0</v>
@@ -4861,10 +4861,10 @@
         <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
@@ -4938,10 +4938,10 @@
         <v>47</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E22" s="4">
         <v>0</v>
@@ -5015,10 +5015,10 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E23" s="4">
         <v>0</v>
@@ -5092,10 +5092,10 @@
         <v>47</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="E24" s="4">
         <v>0</v>
@@ -5169,10 +5169,10 @@
         <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E25" s="4">
         <v>0</v>
@@ -5246,10 +5246,10 @@
         <v>47</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="E26" s="4">
         <v>0</v>
@@ -5323,10 +5323,10 @@
         <v>47</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
@@ -5400,7 +5400,7 @@
         <v>47</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>3</v>
@@ -5477,10 +5477,10 @@
         <v>47</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="E29" s="4">
         <v>0</v>
@@ -5554,10 +5554,10 @@
         <v>47</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="E30" s="4">
         <v>0</v>

</xml_diff>